<commit_message>
add validations to model artist
</commit_message>
<xml_diff>
--- a/ERD.xlsx
+++ b/ERD.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>USER</t>
   </si>
@@ -73,28 +73,22 @@
     <t>belongs_to :user</t>
   </si>
   <si>
-    <t>belong_to :artist</t>
-  </si>
-  <si>
     <t>Associations</t>
   </si>
   <si>
-    <t>has_many :artists, through :concert</t>
-  </si>
-  <si>
-    <t>has_many :users, through :concert</t>
-  </si>
-  <si>
-    <t>photo:</t>
-  </si>
-  <si>
-    <t>image url</t>
-  </si>
-  <si>
     <t>name(unique):</t>
   </si>
   <si>
     <t>Date.time</t>
+  </si>
+  <si>
+    <t>has_many :artists</t>
+  </si>
+  <si>
+    <t>similar artist:</t>
+  </si>
+  <si>
+    <t>imgage url</t>
   </si>
 </sst>
 </file>
@@ -333,7 +327,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -422,6 +416,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -629,16 +629,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>863600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>378460</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>10160</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -647,8 +647,53 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8966200" y="1333500"/>
-          <a:ext cx="10160" cy="1343660"/>
+          <a:off x="2082800" y="787400"/>
+          <a:ext cx="3403600" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Connector 25"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4648200" y="1041400"/>
+          <a:ext cx="825500" cy="165100"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -676,59 +721,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="26" name="Straight Connector 25"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6959600" y="2489200"/>
-          <a:ext cx="825500" cy="165100"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -737,53 +737,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6972300" y="2692400"/>
-          <a:ext cx="838200" cy="177800"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="28" name="Straight Connector 27"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6921500" y="2654300"/>
-          <a:ext cx="2044700" cy="12700"/>
+          <a:off x="4660900" y="901700"/>
+          <a:ext cx="800100" cy="127000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1135,7 +1090,7 @@
   <dimension ref="A3:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="E12" sqref="E12:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1184,7 +1139,7 @@
         <v>4</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>4</v>
@@ -1200,12 +1155,21 @@
         <v>4</v>
       </c>
       <c r="H7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="H8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="9"/>
+      <c r="I8" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="35"/>
     </row>
     <row r="9" spans="1:10">
       <c r="E9" s="6"/>
@@ -1244,7 +1208,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
@@ -1287,7 +1251,7 @@
     </row>
     <row r="20" spans="1:6" ht="20">
       <c r="A20" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
@@ -1304,7 +1268,7 @@
     </row>
     <row r="22" spans="1:6" ht="16" customHeight="1">
       <c r="A22" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -1331,7 +1295,7 @@
     </row>
     <row r="25" spans="1:6" ht="16" customHeight="1">
       <c r="A25" s="17" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
@@ -1339,9 +1303,7 @@
       <c r="E25" s="14"/>
     </row>
     <row r="26" spans="1:6" ht="16" customHeight="1">
-      <c r="A26" s="21" t="s">
-        <v>15</v>
-      </c>
+      <c r="A26" s="21"/>
       <c r="B26" s="22"/>
       <c r="C26" s="15"/>
       <c r="D26" s="16"/>
@@ -1366,21 +1328,20 @@
       <c r="E28" s="15"/>
     </row>
     <row r="29" spans="1:6" ht="16" customHeight="1">
-      <c r="A29" s="25" t="s">
-        <v>17</v>
-      </c>
+      <c r="A29" s="25"/>
       <c r="B29" s="26"/>
       <c r="C29" s="26"/>
       <c r="D29" s="27"/>
       <c r="E29" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
     <mergeCell ref="A29:C29"/>
     <mergeCell ref="A25:D25"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I8:J8"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="A23:D23"/>

</xml_diff>